<commit_message>
vowels test on 15 languages base
</commit_message>
<xml_diff>
--- a/src/main/java/input/Input.xlsx
+++ b/src/main/java/input/Input.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="298">
   <si>
     <t>Languages</t>
   </si>
@@ -293,6 +294,621 @@
   </si>
   <si>
     <t>leŋ</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>horn</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>rain</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>nose</t>
+  </si>
+  <si>
+    <t>heart</t>
+  </si>
+  <si>
+    <t>Lokono</t>
+  </si>
+  <si>
+    <t>hoɽaɽo</t>
+  </si>
+  <si>
+    <t>kǝɾa</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>motʰoko</t>
+  </si>
+  <si>
+    <t>šiɾi</t>
+  </si>
+  <si>
+    <t>wašina</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>awaduli</t>
+  </si>
+  <si>
+    <t>šiba</t>
+  </si>
+  <si>
+    <t>bana</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>koa</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>kutʸi</t>
+  </si>
+  <si>
+    <t>amukʸiˈun</t>
+  </si>
+  <si>
+    <t>yopˈok</t>
+  </si>
+  <si>
+    <t>m̊iɲaŋ=pˈǝ</t>
+  </si>
+  <si>
+    <t>umiˈaŋ</t>
+  </si>
+  <si>
+    <t>ǝmbuɾˈu</t>
+  </si>
+  <si>
+    <t>žin</t>
+  </si>
+  <si>
+    <t>tetˈun</t>
+  </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>Krenak</t>
+  </si>
+  <si>
+    <t>takɾˈuk</t>
+  </si>
+  <si>
+    <t>žǝt</t>
+  </si>
+  <si>
+    <t>iŋgˈu</t>
+  </si>
+  <si>
+    <t>nǯuwˈem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q'eqchi' </t>
+  </si>
+  <si>
+    <t>čoq</t>
+  </si>
+  <si>
+    <t>xe’</t>
+  </si>
+  <si>
+    <t>hab’</t>
+  </si>
+  <si>
+    <t>samahi’</t>
+  </si>
+  <si>
+    <t>iq’</t>
+  </si>
+  <si>
+    <t>u’uj</t>
+  </si>
+  <si>
+    <t>č'ool</t>
+  </si>
+  <si>
+    <t>oq</t>
+  </si>
+  <si>
+    <t>pek</t>
+  </si>
+  <si>
+    <t>xaq</t>
+  </si>
+  <si>
+    <t>mol</t>
+  </si>
+  <si>
+    <t>xukub'</t>
+  </si>
+  <si>
+    <t>abˈik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ˈela  </t>
+  </si>
+  <si>
+    <t>abˈiʔe</t>
+  </si>
+  <si>
+    <t>ˈegaɬ</t>
+  </si>
+  <si>
+    <t>Highland Chontal</t>
+  </si>
+  <si>
+    <t>ummˈa-way</t>
+  </si>
+  <si>
+    <t>ˈime</t>
+  </si>
+  <si>
+    <t>gwi</t>
+  </si>
+  <si>
+    <t>ibˈi=macʼ</t>
+  </si>
+  <si>
+    <t>ˈawaʔ</t>
+  </si>
+  <si>
+    <t>ʔnaɬ</t>
+  </si>
+  <si>
+    <t>onšˈa-hmaʔ</t>
+  </si>
+  <si>
+    <t>ʔmis</t>
+  </si>
+  <si>
+    <t>lˈupːu</t>
+  </si>
+  <si>
+    <t>kˈolːi</t>
+  </si>
+  <si>
+    <t>pˈuːlu</t>
+  </si>
+  <si>
+    <t>kˈilːi</t>
+  </si>
+  <si>
+    <t>ʔˈilaw</t>
+  </si>
+  <si>
+    <t>hˈulːu</t>
+  </si>
+  <si>
+    <t>ʔˈupːa</t>
+  </si>
+  <si>
+    <t>ʂˈukuy</t>
+  </si>
+  <si>
+    <t>kˈiwel</t>
+  </si>
+  <si>
+    <t>hˈuːk</t>
+  </si>
+  <si>
+    <t>wˈuʂki</t>
+  </si>
+  <si>
+    <t>kˈo</t>
+  </si>
+  <si>
+    <t>Bodega Miwok</t>
+  </si>
+  <si>
+    <t>hošonti</t>
+  </si>
+  <si>
+    <t>akaštala</t>
+  </si>
+  <si>
+    <t>umba</t>
+  </si>
+  <si>
+    <t>šinuk</t>
+  </si>
+  <si>
+    <t>mahli</t>
+  </si>
+  <si>
+    <t>ibichilu</t>
+  </si>
+  <si>
+    <t>čuǝš</t>
+  </si>
+  <si>
+    <t>iyyi</t>
+  </si>
+  <si>
+    <t>təl</t>
+  </si>
+  <si>
+    <t>hish</t>
+  </si>
+  <si>
+    <t>ush</t>
+  </si>
+  <si>
+    <t>lapish</t>
+  </si>
+  <si>
+    <t>Choctaw</t>
+  </si>
+  <si>
+    <t>šaːr</t>
+  </si>
+  <si>
+    <t>tas</t>
+  </si>
+  <si>
+    <t>ir-o</t>
+  </si>
+  <si>
+    <t>fuːt-u</t>
+  </si>
+  <si>
+    <t>sir</t>
+  </si>
+  <si>
+    <t>siy</t>
+  </si>
+  <si>
+    <t>nib</t>
+  </si>
+  <si>
+    <t>org-o</t>
+  </si>
+  <si>
+    <t>šūʔ-ā</t>
+  </si>
+  <si>
+    <t>Yem</t>
+  </si>
+  <si>
+    <t>tòš-à</t>
+  </si>
+  <si>
+    <t>kēw-ā</t>
+  </si>
+  <si>
+    <t>kàl-ā</t>
+  </si>
+  <si>
+    <t>dama</t>
+  </si>
+  <si>
+    <t>tixa</t>
+  </si>
+  <si>
+    <t>saːsı-ma</t>
+  </si>
+  <si>
+    <t>zuba</t>
+  </si>
+  <si>
+    <t>ita</t>
+  </si>
+  <si>
+    <t>kʼubica</t>
+  </si>
+  <si>
+    <t>ɕogwa</t>
+  </si>
+  <si>
+    <t>dyukwa</t>
+  </si>
+  <si>
+    <t>iša</t>
+  </si>
+  <si>
+    <t>cʼidya</t>
+  </si>
+  <si>
+    <t>gıša</t>
+  </si>
+  <si>
+    <t>nasob</t>
+  </si>
+  <si>
+    <t>tɛrb-i</t>
+  </si>
+  <si>
+    <t>hala</t>
+  </si>
+  <si>
+    <t>lugʋd</t>
+  </si>
+  <si>
+    <t>šımal</t>
+  </si>
+  <si>
+    <t>dǝmmo</t>
+  </si>
+  <si>
+    <t>asıma</t>
+  </si>
+  <si>
+    <t>bǝla</t>
+  </si>
+  <si>
+    <t>Sai Gumuz</t>
+  </si>
+  <si>
+    <t>Nara</t>
+  </si>
+  <si>
+    <t>t̪ana</t>
+  </si>
+  <si>
+    <t>tıfinī</t>
+  </si>
+  <si>
+    <t>war-i</t>
+  </si>
+  <si>
+    <t>keːl-i</t>
+  </si>
+  <si>
+    <t>Ko</t>
+  </si>
+  <si>
+    <t>ibʷɔɽua</t>
+  </si>
+  <si>
+    <t>ʋndalia</t>
+  </si>
+  <si>
+    <t>rǝmʷa</t>
+  </si>
+  <si>
+    <t>eːβia</t>
+  </si>
+  <si>
+    <t>βɛːra</t>
+  </si>
+  <si>
+    <t>aðɔla</t>
+  </si>
+  <si>
+    <t>ufuða</t>
+  </si>
+  <si>
+    <t>ð=imaniɲa</t>
+  </si>
+  <si>
+    <t>l=ɔ́ándrá</t>
+  </si>
+  <si>
+    <t>ð=àt̪áy</t>
+  </si>
+  <si>
+    <t>l=ɛ́ɲá</t>
+  </si>
+  <si>
+    <t>θál</t>
+  </si>
+  <si>
+    <t>ʓru</t>
+  </si>
+  <si>
+    <t>lika</t>
+  </si>
+  <si>
+    <t>mĩdi</t>
+  </si>
+  <si>
+    <t>ŋkriã</t>
+  </si>
+  <si>
+    <t>lifa</t>
+  </si>
+  <si>
+    <t>wɔ</t>
+  </si>
+  <si>
+    <t>bo-lʋwı</t>
+  </si>
+  <si>
+    <t>lı=ka</t>
+  </si>
+  <si>
+    <t>Abidji</t>
+  </si>
+  <si>
+    <t>áhʋ́á</t>
+  </si>
+  <si>
+    <t>ń=dî</t>
+  </si>
+  <si>
+    <t>rʋ́wà</t>
+  </si>
+  <si>
+    <t>lú=bóbú</t>
+  </si>
+  <si>
+    <t>Ket</t>
+  </si>
+  <si>
+    <t>ˈasʸpulʸ</t>
+  </si>
+  <si>
+    <t>tirʸ</t>
+  </si>
+  <si>
+    <t>ˈulʸ-esʸ</t>
+  </si>
+  <si>
+    <t>hˈɜnʸaŋ</t>
+  </si>
+  <si>
+    <t>bey</t>
+  </si>
+  <si>
+    <t>ˈɔlɨn</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>bu-lʸ</t>
+  </si>
+  <si>
+    <t>ɜː</t>
+  </si>
+  <si>
+    <t>ɛʔy</t>
+  </si>
+  <si>
+    <t>qɔʔ</t>
+  </si>
+  <si>
+    <t>tɨʔsʸ</t>
+  </si>
+  <si>
+    <t>peɬǝŋ</t>
+  </si>
+  <si>
+    <t>ɬort</t>
+  </si>
+  <si>
+    <t>yom</t>
+  </si>
+  <si>
+    <t>saŋkɨː</t>
+  </si>
+  <si>
+    <t>wɔːt</t>
+  </si>
+  <si>
+    <t>ɲoɬ</t>
+  </si>
+  <si>
+    <t>sem</t>
+  </si>
+  <si>
+    <t>kör</t>
+  </si>
+  <si>
+    <t>Юганский хантыйский</t>
+  </si>
+  <si>
+    <t xml:space="preserve">käw  </t>
+  </si>
+  <si>
+    <t>ɭɨːpǝ̆t</t>
+  </si>
+  <si>
+    <t>moːk</t>
+  </si>
+  <si>
+    <t>ɔːŋǝ̆t</t>
+  </si>
+  <si>
+    <t>aso-y</t>
+  </si>
+  <si>
+    <t>tum</t>
+  </si>
+  <si>
+    <t>aʁa-la</t>
+  </si>
+  <si>
+    <t>qːum</t>
+  </si>
+  <si>
+    <t>muš</t>
+  </si>
+  <si>
+    <t>boχˤmoʁ</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>tur</t>
+  </si>
+  <si>
+    <t>Nidzh Udi</t>
+  </si>
+  <si>
+    <t>χazal</t>
+  </si>
+  <si>
+    <t>qokːla</t>
+  </si>
+  <si>
+    <t>muqːʕa</t>
+  </si>
+  <si>
+    <t>žˤe</t>
+  </si>
+  <si>
+    <t>wahawaha</t>
+  </si>
+  <si>
+    <t>ikiʔiki</t>
+  </si>
+  <si>
+    <t>uːta</t>
+  </si>
+  <si>
+    <t>oːne</t>
+  </si>
+  <si>
+    <t>oːru</t>
+  </si>
+  <si>
+    <t>pano-na</t>
+  </si>
+  <si>
+    <t>rae-na</t>
+  </si>
+  <si>
+    <t>aʔe-na</t>
+  </si>
+  <si>
+    <t>Are'are (Waiahaa)</t>
+  </si>
+  <si>
+    <t>hau</t>
+  </si>
+  <si>
+    <t>poʔere</t>
+  </si>
+  <si>
+    <t>apota</t>
   </si>
 </sst>
 </file>
@@ -308,15 +924,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -324,11 +958,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +1129,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -643,10 +1468,694 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="L16" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="M16" s="35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
obstruent and stops fixes
</commit_message>
<xml_diff>
--- a/src/main/java/input/Input.xlsx
+++ b/src/main/java/input/Input.xlsx
@@ -207,9 +207,6 @@
     <t>t̪ana</t>
   </si>
   <si>
-    <t>tıfinī</t>
-  </si>
-  <si>
     <t>war-i</t>
   </si>
   <si>
@@ -561,30 +558,6 @@
     <t>Gurindji</t>
   </si>
   <si>
-    <t>šūʔ-ā</t>
-  </si>
-  <si>
-    <t>tòš-à</t>
-  </si>
-  <si>
-    <t>kēw-ā</t>
-  </si>
-  <si>
-    <t>kàl-ā</t>
-  </si>
-  <si>
-    <t>lú=bóbú</t>
-  </si>
-  <si>
-    <t>rʋ́wà</t>
-  </si>
-  <si>
-    <t>ń=dî</t>
-  </si>
-  <si>
-    <t>áhʋ́á</t>
-  </si>
-  <si>
     <t>kʰvɑ</t>
   </si>
   <si>
@@ -787,6 +760,33 @@
   </si>
   <si>
     <t>jamana</t>
+  </si>
+  <si>
+    <t>šuʔ-a</t>
+  </si>
+  <si>
+    <t>toš-a</t>
+  </si>
+  <si>
+    <t>kew-a</t>
+  </si>
+  <si>
+    <t>kal-a</t>
+  </si>
+  <si>
+    <t>rʋwa</t>
+  </si>
+  <si>
+    <t>lu=bobu</t>
+  </si>
+  <si>
+    <t>ahʋa</t>
+  </si>
+  <si>
+    <t>n=di</t>
+  </si>
+  <si>
+    <t>tıfini</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>24</v>
@@ -1567,16 +1567,16 @@
         <v>51</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>183</v>
+        <v>250</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>184</v>
+        <v>251</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>43</v>
@@ -1611,13 +1611,13 @@
         <v>62</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>52</v>
@@ -1646,404 +1646,404 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>185</v>
+        <v>253</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>186</v>
+        <v>252</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>187</v>
+        <v>255</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="F6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M6" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="I7" s="57" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="L7" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="M7" s="58" t="s">
         <v>191</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="G7" s="57" t="s">
-        <v>194</v>
-      </c>
-      <c r="H7" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="I7" s="57" t="s">
-        <v>196</v>
-      </c>
-      <c r="J7" s="57" t="s">
-        <v>197</v>
-      </c>
-      <c r="K7" s="57" t="s">
-        <v>198</v>
-      </c>
-      <c r="L7" s="57" t="s">
-        <v>199</v>
-      </c>
-      <c r="M7" s="58" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="D8" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>112</v>
-      </c>
       <c r="F8" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="H8" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="I8" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="M8" s="22" t="s">
         <v>107</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="49" t="s">
+      <c r="G9" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="H9" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="I9" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="J9" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="K9" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="L9" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="49" t="s">
+      <c r="M9" s="55" t="s">
         <v>94</v>
-      </c>
-      <c r="M9" s="55" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="50" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="I10" s="50" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="J10" s="50" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="K10" s="50" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="L10" s="50" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="M10" s="53" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="K11" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="L11" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="M11" s="48" t="s">
         <v>214</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="J11" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="K11" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="L11" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="M11" s="48" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="K12" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="L12" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="M12" s="26" t="s">
         <v>226</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="M12" s="26" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="22" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="C14" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="D14" s="28" t="s">
         <v>124</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>125</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="H14" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="I14" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="J14" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="K14" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="L14" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="M14" s="31" t="s">
         <v>120</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="L15" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="M15" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2071,10 +2071,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2082,11 +2082,11 @@
         <v>11</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="40"/>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,11 +2094,11 @@
         <v>14</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="40"/>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="40"/>
     </row>
@@ -2115,11 +2115,11 @@
         <v>28</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="40"/>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="40"/>
     </row>
@@ -2136,7 +2136,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" s="40"/>
     </row>
@@ -2145,7 +2145,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="40"/>
     </row>
@@ -2154,11 +2154,11 @@
         <v>60</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="40"/>
       <c r="E9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2166,65 +2166,65 @@
         <v>61</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" s="40"/>
       <c r="E10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" t="s">
         <v>169</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="E12" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="40"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" s="40"/>
     </row>
@@ -2286,43 +2286,43 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="F21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="I21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="J21" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="K21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="L21" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="L21" s="17" t="s">
+      <c r="M21" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2401,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -2410,10 +2410,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>127</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2421,10 +2421,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,10 +2432,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,10 +2443,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2454,13 +2454,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
         <v>135</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,10 +2468,10 @@
         <v>42</v>
       </c>
       <c r="B7" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>138</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,10 +2479,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>141</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,13 +2490,13 @@
         <v>60</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" t="s">
         <v>144</v>
-      </c>
-      <c r="D9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,79 +2504,79 @@
         <v>61</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="D12" t="s">
         <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="37" t="s">
         <v>155</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>157</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all phonemes count, unknown phonemes, empty symb in transcription fixed
</commit_message>
<xml_diff>
--- a/src/main/java/input/Input.xlsx
+++ b/src/main/java/input/Input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="387">
   <si>
     <t>Languages</t>
   </si>
@@ -787,6 +787,396 @@
   </si>
   <si>
     <t>tıfini</t>
+  </si>
+  <si>
+    <t>Nuer</t>
+  </si>
+  <si>
+    <t>pam</t>
+  </si>
+  <si>
+    <t>ʓit</t>
+  </si>
+  <si>
+    <t>tuɔŋ</t>
+  </si>
+  <si>
+    <t>tuŋ</t>
+  </si>
+  <si>
+    <t>puaːr</t>
+  </si>
+  <si>
+    <t>mie-t̪</t>
+  </si>
+  <si>
+    <t>n̪ial</t>
+  </si>
+  <si>
+    <t>lied</t>
+  </si>
+  <si>
+    <t>ʓiɔm</t>
+  </si>
+  <si>
+    <t>wum</t>
+  </si>
+  <si>
+    <t>lɔc</t>
+  </si>
+  <si>
+    <t>coɣ</t>
+  </si>
+  <si>
+    <t>Fur</t>
+  </si>
+  <si>
+    <t>d˗ido</t>
+  </si>
+  <si>
+    <t>d˗ɛlma˗ŋ</t>
+  </si>
+  <si>
+    <t>dirɔ</t>
+  </si>
+  <si>
+    <t>d˗ɔlba</t>
+  </si>
+  <si>
+    <t>kutu</t>
+  </si>
+  <si>
+    <t>d˗iːjiŋ</t>
+  </si>
+  <si>
+    <t>kui</t>
+  </si>
+  <si>
+    <t>ŋaiɲ</t>
+  </si>
+  <si>
+    <t>daulu</t>
+  </si>
+  <si>
+    <t>dɔrmi</t>
+  </si>
+  <si>
+    <t>kilma</t>
+  </si>
+  <si>
+    <t>tar</t>
+  </si>
+  <si>
+    <t>Daza</t>
+  </si>
+  <si>
+    <t>ji</t>
+  </si>
+  <si>
+    <t>kɔllu</t>
+  </si>
+  <si>
+    <t>šili</t>
+  </si>
+  <si>
+    <t>jaɛ</t>
+  </si>
+  <si>
+    <t>kiri</t>
+  </si>
+  <si>
+    <t>ḍjulu</t>
+  </si>
+  <si>
+    <t>ḍɔo</t>
+  </si>
+  <si>
+    <t>anɛšɛ</t>
+  </si>
+  <si>
+    <t>awɔnɔ</t>
+  </si>
+  <si>
+    <t>čalula</t>
+  </si>
+  <si>
+    <t>awɔr</t>
+  </si>
+  <si>
+    <t>gɔḍɔgɔḍɔ</t>
+  </si>
+  <si>
+    <t>Afitti</t>
+  </si>
+  <si>
+    <t>mbǝrɛ</t>
+  </si>
+  <si>
+    <t>laluwa</t>
+  </si>
+  <si>
+    <t>domi</t>
+  </si>
+  <si>
+    <t>gwurt̪un</t>
+  </si>
+  <si>
+    <t>leʓa</t>
+  </si>
+  <si>
+    <t>kuru</t>
+  </si>
+  <si>
+    <t>arǝŋga</t>
+  </si>
+  <si>
+    <t>sua</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>ŋwut̪a</t>
+  </si>
+  <si>
+    <t>t̪ilim</t>
+  </si>
+  <si>
+    <t>magila</t>
+  </si>
+  <si>
+    <t>Ik</t>
+  </si>
+  <si>
+    <t>ɠwas</t>
+  </si>
+  <si>
+    <t>kakʰ</t>
+  </si>
+  <si>
+    <t>ˈɓiƥḁ</t>
+  </si>
+  <si>
+    <t>ɛƥḁ</t>
+  </si>
+  <si>
+    <t>ɡoʒo</t>
+  </si>
+  <si>
+    <t>ˈsɔkḁ</t>
+  </si>
+  <si>
+    <t>didi</t>
+  </si>
+  <si>
+    <t>ʄumuʄumas</t>
+  </si>
+  <si>
+    <t>suɡur</t>
+  </si>
+  <si>
+    <t>akʼat</t>
+  </si>
+  <si>
+    <t>ɡur</t>
+  </si>
+  <si>
+    <t>dea</t>
+  </si>
+  <si>
+    <t>Tennet</t>
+  </si>
+  <si>
+    <t>ɓɛ</t>
+  </si>
+  <si>
+    <t>vʌrʌɲo-č</t>
+  </si>
+  <si>
+    <t>ɓʋrʋ</t>
+  </si>
+  <si>
+    <t>otːo-n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɗiið </t>
+  </si>
+  <si>
+    <t>egːero-č</t>
+  </si>
+  <si>
+    <t>tamːu</t>
+  </si>
+  <si>
+    <t>ʌðʌ-č</t>
+  </si>
+  <si>
+    <t>ŋɔt</t>
+  </si>
+  <si>
+    <t>ʋŋɛ-č</t>
+  </si>
+  <si>
+    <t>ðını-n</t>
+  </si>
+  <si>
+    <t>ðo-č</t>
+  </si>
+  <si>
+    <t>Midob</t>
+  </si>
+  <si>
+    <t>ull-i</t>
+  </si>
+  <si>
+    <t>pi-di</t>
+  </si>
+  <si>
+    <t>ayi-di</t>
+  </si>
+  <si>
+    <t>kǝːɕ-i</t>
+  </si>
+  <si>
+    <t>teɕɕi-di</t>
+  </si>
+  <si>
+    <t>ir-di</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>uku-di</t>
+  </si>
+  <si>
+    <t>essi</t>
+  </si>
+  <si>
+    <t>eseŋi</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>os-e</t>
+  </si>
+  <si>
+    <t>Seri</t>
+  </si>
+  <si>
+    <t>ʔast</t>
+  </si>
+  <si>
+    <t>i=stx</t>
+  </si>
+  <si>
+    <t>iː=pχ</t>
+  </si>
+  <si>
+    <t>i=tˈaːmaɬka</t>
+  </si>
+  <si>
+    <t>ʔˈoːka-ɬa</t>
+  </si>
+  <si>
+    <t>χˈaːi</t>
+  </si>
+  <si>
+    <t>ˈi=pka</t>
+  </si>
+  <si>
+    <t>ʔamt</t>
+  </si>
+  <si>
+    <t>ʔai</t>
+  </si>
+  <si>
+    <t>iiɸ</t>
+  </si>
+  <si>
+    <t>moš</t>
+  </si>
+  <si>
+    <t>i=tˈoaː</t>
+  </si>
+  <si>
+    <t>Cocopa</t>
+  </si>
+  <si>
+    <t>xuːɾ</t>
+  </si>
+  <si>
+    <t>wal</t>
+  </si>
+  <si>
+    <t>məšəʔop</t>
+  </si>
+  <si>
+    <t>nyiqwah</t>
+  </si>
+  <si>
+    <t>ʔiqwi</t>
+  </si>
+  <si>
+    <t>šma</t>
+  </si>
+  <si>
+    <t>paj</t>
+  </si>
+  <si>
+    <t>mačʔa</t>
+  </si>
+  <si>
+    <t>tyʔihaj</t>
+  </si>
+  <si>
+    <t>njixu</t>
+  </si>
+  <si>
+    <t>njiwey</t>
+  </si>
+  <si>
+    <t>njimi</t>
+  </si>
+  <si>
+    <t>Hopi</t>
+  </si>
+  <si>
+    <t>ʔowa</t>
+  </si>
+  <si>
+    <t>nahpi</t>
+  </si>
+  <si>
+    <t>nøhɨ</t>
+  </si>
+  <si>
+    <t>a:la</t>
+  </si>
+  <si>
+    <t>ʔomawɨ</t>
+  </si>
+  <si>
+    <t>naʔat</t>
+  </si>
+  <si>
+    <t>jo:jaŋw</t>
+  </si>
+  <si>
+    <t>tɨ:wa</t>
+  </si>
+  <si>
+    <t>hɨ:kaŋwɨ</t>
+  </si>
+  <si>
+    <t>jaqa</t>
+  </si>
+  <si>
+    <t>unaŋwa</t>
+  </si>
+  <si>
+    <t>kɨkɨ</t>
   </si>
 </sst>
 </file>
@@ -810,7 +1200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -835,8 +1225,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFC9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -978,17 +1374,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1005,7 +1390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1038,10 +1423,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1068,7 +1451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1111,6 +1493,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1416,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1911,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
@@ -1689,40 +2078,40 @@
       <c r="A7" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="H7" s="57" t="s">
+      <c r="H7" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="J7" s="57" t="s">
+      <c r="J7" s="54" t="s">
         <v>188</v>
       </c>
-      <c r="K7" s="57" t="s">
+      <c r="K7" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="L7" s="57" t="s">
+      <c r="L7" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="M7" s="58" t="s">
+      <c r="M7" s="55" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1730,7 +2119,7 @@
       <c r="A8" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>112</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -1771,40 +2160,40 @@
       <c r="A9" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="I9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="J9" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="K9" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="L9" s="49" t="s">
+      <c r="L9" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="55" t="s">
+      <c r="M9" s="52" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1812,38 +2201,38 @@
       <c r="A10" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50" t="s">
+      <c r="F10" s="47"/>
+      <c r="G10" s="47" t="s">
         <v>196</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="K10" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="M10" s="53" t="s">
+      <c r="M10" s="50" t="s">
         <v>202</v>
       </c>
     </row>
@@ -1851,40 +2240,40 @@
       <c r="A11" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="K11" s="46" t="s">
+      <c r="K11" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="L11" s="47" t="s">
+      <c r="L11" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="M11" s="48" t="s">
+      <c r="M11" s="45" t="s">
         <v>214</v>
       </c>
     </row>
@@ -1930,86 +2319,86 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22" t="s">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="5" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="M14" s="26" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="60" t="s">
         <v>237</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2044,6 +2433,416 @@
       </c>
       <c r="M15" s="5" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="58" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>307</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>325</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>326</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="L21" s="59" t="s">
+        <v>333</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="61" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>342</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="M22" s="41" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
+        <v>361</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="M25" s="41" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -2081,10 +2880,10 @@
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="38"/>
       <c r="E2" t="s">
         <v>164</v>
       </c>
@@ -2093,10 +2892,10 @@
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="38"/>
       <c r="E3" t="s">
         <v>164</v>
       </c>
@@ -2105,19 +2904,19 @@
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="40"/>
+      <c r="C5" s="38"/>
       <c r="E5" t="s">
         <v>170</v>
       </c>
@@ -2126,37 +2925,37 @@
       <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="38"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="38"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="38"/>
       <c r="E9" t="s">
         <v>169</v>
       </c>
@@ -2165,10 +2964,10 @@
       <c r="A10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="38"/>
       <c r="E10" t="s">
         <v>172</v>
       </c>
@@ -2177,17 +2976,17 @@
       <c r="A11" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="38" t="s">
         <v>165</v>
       </c>
       <c r="E12" t="s">
@@ -2195,38 +2994,38 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="38"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="38"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2409,10 +3208,10 @@
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="34" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2420,10 +3219,10 @@
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2431,10 +3230,10 @@
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="35" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2442,10 +3241,10 @@
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2453,10 +3252,10 @@
       <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>136</v>
       </c>
       <c r="D6" t="s">
@@ -2467,10 +3266,10 @@
       <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2478,10 +3277,10 @@
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2489,10 +3288,10 @@
       <c r="A9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>143</v>
       </c>
       <c r="D9" t="s">
@@ -2503,7 +3302,7 @@
       <c r="A10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>142</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2514,7 +3313,7 @@
       <c r="A11" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2525,10 +3324,10 @@
       <c r="A12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>149</v>
       </c>
       <c r="D12" t="s">
@@ -2536,13 +3335,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2550,10 +3349,10 @@
       <c r="A14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="34" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2561,21 +3360,21 @@
       <c r="A15" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="35" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="30" t="s">
         <v>121</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="34" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
5 more Niger-Congo langs
</commit_message>
<xml_diff>
--- a/src/main/java/input/Input.xlsx
+++ b/src/main/java/input/Input.xlsx
@@ -10,13 +10,14 @@
     <sheet name="InputWords" sheetId="2" r:id="rId1"/>
     <sheet name="LangPhonetics" sheetId="1" r:id="rId2"/>
     <sheet name="LangGeneology" sheetId="3" r:id="rId3"/>
+    <sheet name="Geneology" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="570">
   <si>
     <t>Languages</t>
   </si>
@@ -1450,13 +1451,289 @@
   </si>
   <si>
     <t>wata</t>
+  </si>
+  <si>
+    <t>Niger-Congo</t>
+  </si>
+  <si>
+    <t>Mande</t>
+  </si>
+  <si>
+    <t>Dogon</t>
+  </si>
+  <si>
+    <t>Ijoid</t>
+  </si>
+  <si>
+    <t>Bangime</t>
+  </si>
+  <si>
+    <t>Siamon</t>
+  </si>
+  <si>
+    <t>KORDOFANIAN</t>
+  </si>
+  <si>
+    <t>Atlantic-Congo</t>
+  </si>
+  <si>
+    <t>Atlantic</t>
+  </si>
+  <si>
+    <t>Senegambian</t>
+  </si>
+  <si>
+    <t>Bak</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Limba</t>
+  </si>
+  <si>
+    <t>Gola</t>
+  </si>
+  <si>
+    <t>Volta-Congo</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Savannas</t>
+  </si>
+  <si>
+    <t>Kru</t>
+  </si>
+  <si>
+    <t>Senufo</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Kwa</t>
+  </si>
+  <si>
+    <t>Volta-Niger</t>
+  </si>
+  <si>
+    <t>Benue-Congo</t>
+  </si>
+  <si>
+    <t>Bantoid-Cross</t>
+  </si>
+  <si>
+    <t>Central Nigerian</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>Cross-River</t>
+  </si>
+  <si>
+    <t>Bantoid</t>
+  </si>
+  <si>
+    <t>Bantu</t>
+  </si>
+  <si>
+    <t>Gur</t>
+  </si>
+  <si>
+    <t>Ubangian</t>
+  </si>
+  <si>
+    <t>etc</t>
+  </si>
+  <si>
+    <t>Noon</t>
+  </si>
+  <si>
+    <t>atox</t>
+  </si>
+  <si>
+    <t>pʊʔ</t>
+  </si>
+  <si>
+    <t>wak</t>
+  </si>
+  <si>
+    <t>yit</t>
+  </si>
+  <si>
+    <t>ɲaižol</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>toʷ</t>
+  </si>
+  <si>
+    <t>kolɛɲ</t>
+  </si>
+  <si>
+    <t>ʊris</t>
+  </si>
+  <si>
+    <t>kuluŋɲon</t>
+  </si>
+  <si>
+    <t>qot</t>
+  </si>
+  <si>
+    <t>Baka</t>
+  </si>
+  <si>
+    <t>kpa˗</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>kɛnǯɛ</t>
+  </si>
+  <si>
+    <t>temɛ</t>
+  </si>
+  <si>
+    <t>Sherbro</t>
+  </si>
+  <si>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>suːŋ</t>
+  </si>
+  <si>
+    <t>gbɔl</t>
+  </si>
+  <si>
+    <t>Degema</t>
+  </si>
+  <si>
+    <t>ohiŋʷ</t>
+  </si>
+  <si>
+    <t>ʊɓi</t>
+  </si>
+  <si>
+    <t>ukije</t>
+  </si>
+  <si>
+    <t>ʊkpan</t>
+  </si>
+  <si>
+    <t>oɓutu</t>
+  </si>
+  <si>
+    <t>ʊsɪnɛ</t>
+  </si>
+  <si>
+    <t>ɔkpar</t>
+  </si>
+  <si>
+    <t>ʊkpɛkpilɛm</t>
+  </si>
+  <si>
+    <t>isußeɲ</t>
+  </si>
+  <si>
+    <t>ʊɳʷɔißom</t>
+  </si>
+  <si>
+    <t>aßi</t>
+  </si>
+  <si>
+    <t>nono</t>
+  </si>
+  <si>
+    <t>bəŋ</t>
+  </si>
+  <si>
+    <t>ɓaŋa˗bo</t>
+  </si>
+  <si>
+    <t>liwɛwɛ</t>
+  </si>
+  <si>
+    <t>siesie</t>
+  </si>
+  <si>
+    <t>saŋu</t>
+  </si>
+  <si>
+    <t>papala</t>
+  </si>
+  <si>
+    <t>timi</t>
+  </si>
+  <si>
+    <t>pɔm</t>
+  </si>
+  <si>
+    <t>d˗epel</t>
+  </si>
+  <si>
+    <t>tʰọk˗a˗tʰọk</t>
+  </si>
+  <si>
+    <t>nteŋk</t>
+  </si>
+  <si>
+    <t>hwɛ</t>
+  </si>
+  <si>
+    <t>həŋ</t>
+  </si>
+  <si>
+    <t>min kunɛ</t>
+  </si>
+  <si>
+    <t>Bambara</t>
+  </si>
+  <si>
+    <t>ŋɒŋgɒrɒ</t>
+  </si>
+  <si>
+    <t>fura</t>
+  </si>
+  <si>
+    <t>fan</t>
+  </si>
+  <si>
+    <t>biɲɛ</t>
+  </si>
+  <si>
+    <t>kabanɒgɒ</t>
+  </si>
+  <si>
+    <t>dili</t>
+  </si>
+  <si>
+    <t>čɛnčɛn</t>
+  </si>
+  <si>
+    <t>fiɲɛ</t>
+  </si>
+  <si>
+    <t>nun</t>
+  </si>
+  <si>
+    <t>dusu</t>
+  </si>
+  <si>
+    <t>kontoli</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1495,8 +1772,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1527,8 +1811,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1668,25 +1994,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1694,7 +2007,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1709,10 +2021,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1720,7 +2030,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1789,12 +2098,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1820,22 +2126,78 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2143,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,1270 +2570,1468 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="79" t="s">
+        <v>348</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>374</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="80" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>442</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>443</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>444</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>445</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>446</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>447</v>
+      </c>
+      <c r="J7" s="56" t="s">
+        <v>448</v>
+      </c>
+      <c r="K7" s="56" t="s">
+        <v>449</v>
+      </c>
+      <c r="L7" s="56" t="s">
+        <v>450</v>
+      </c>
+      <c r="M7" s="58" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="K9" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="M9" s="46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="86" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="82" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="J13" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="K13" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="M13" s="51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="87" t="s">
+        <v>387</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>388</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>389</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>391</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="J15" s="59" t="s">
+        <v>396</v>
+      </c>
+      <c r="K15" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>398</v>
+      </c>
+      <c r="M15" s="64" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="88" t="s">
+        <v>400</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>401</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>403</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="G16" s="60" t="s">
+        <v>406</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>408</v>
+      </c>
+      <c r="J16" s="60" t="s">
+        <v>409</v>
+      </c>
+      <c r="K16" s="59" t="s">
+        <v>410</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>411</v>
+      </c>
+      <c r="M16" s="66" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="88" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>414</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>415</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>416</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>417</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>418</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>419</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>420</v>
+      </c>
+      <c r="I17" s="59" t="s">
+        <v>421</v>
+      </c>
+      <c r="J17" s="59" t="s">
+        <v>422</v>
+      </c>
+      <c r="K17" s="59" t="s">
+        <v>423</v>
+      </c>
+      <c r="L17" s="59" t="s">
+        <v>424</v>
+      </c>
+      <c r="M17" s="65" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="88" t="s">
+        <v>426</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>427</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>428</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>429</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>430</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>431</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>432</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>433</v>
+      </c>
+      <c r="I18" s="59" t="s">
+        <v>434</v>
+      </c>
+      <c r="J18" s="59" t="s">
+        <v>435</v>
+      </c>
+      <c r="K18" s="59" t="s">
+        <v>436</v>
+      </c>
+      <c r="L18" s="59" t="s">
+        <v>437</v>
+      </c>
+      <c r="M18" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="88" t="s">
+        <v>452</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>453</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>455</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>456</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>457</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>458</v>
+      </c>
+      <c r="H19" s="59" t="s">
+        <v>459</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="J19" s="59" t="s">
+        <v>461</v>
+      </c>
+      <c r="K19" s="59" t="s">
+        <v>462</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>463</v>
+      </c>
+      <c r="M19" s="66" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
+        <v>465</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>466</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>467</v>
+      </c>
+      <c r="D20" s="62" t="s">
+        <v>468</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>469</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="G20" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="H20" s="62" t="s">
+        <v>472</v>
+      </c>
+      <c r="I20" s="62" t="s">
+        <v>473</v>
+      </c>
+      <c r="J20" s="62" t="s">
+        <v>474</v>
+      </c>
+      <c r="K20" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="L20" s="62" t="s">
+        <v>476</v>
+      </c>
+      <c r="M20" s="67" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="M21" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="81" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="92" t="s">
+        <v>257</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="L23" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="77" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="L26" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>309</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="L28" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="93" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>342</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="M30" s="37" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="94" t="s">
+        <v>510</v>
+      </c>
+      <c r="B31" s="73" t="s">
+        <v>511</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>512</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>513</v>
+      </c>
+      <c r="E31" s="73" t="s">
+        <v>514</v>
+      </c>
+      <c r="F31" s="73" t="s">
+        <v>515</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>516</v>
+      </c>
+      <c r="H31" s="99" t="s">
+        <v>517</v>
+      </c>
+      <c r="I31" s="73" t="s">
+        <v>518</v>
+      </c>
+      <c r="J31" s="73" t="s">
+        <v>519</v>
+      </c>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73" t="s">
+        <v>520</v>
+      </c>
+      <c r="M31" s="74" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="95" t="s">
+        <v>522</v>
+      </c>
+      <c r="B32" s="70" t="s">
+        <v>550</v>
+      </c>
+      <c r="C32" s="70" t="s">
+        <v>523</v>
+      </c>
+      <c r="D32" s="70" t="s">
+        <v>549</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>316</v>
+      </c>
+      <c r="F32" s="70" t="s">
+        <v>548</v>
+      </c>
+      <c r="G32" s="70" t="s">
+        <v>547</v>
+      </c>
+      <c r="H32" s="70" t="s">
+        <v>524</v>
+      </c>
+      <c r="I32" s="70" t="s">
+        <v>525</v>
+      </c>
+      <c r="J32" s="70" t="s">
+        <v>546</v>
+      </c>
+      <c r="K32" s="70" t="s">
+        <v>545</v>
+      </c>
+      <c r="L32" s="70" t="s">
+        <v>526</v>
+      </c>
+      <c r="M32" s="75" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="95" t="s">
+        <v>527</v>
+      </c>
+      <c r="B33" s="70" t="s">
+        <v>528</v>
+      </c>
+      <c r="C33" s="72" t="s">
+        <v>551</v>
+      </c>
+      <c r="D33" s="70" t="s">
+        <v>552</v>
+      </c>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70" t="s">
+        <v>553</v>
+      </c>
+      <c r="G33" s="97" t="s">
+        <v>554</v>
+      </c>
+      <c r="H33" s="70" t="s">
+        <v>555</v>
+      </c>
+      <c r="I33" s="71" t="s">
+        <v>529</v>
+      </c>
+      <c r="J33" s="70" t="s">
+        <v>556</v>
+      </c>
+      <c r="K33" s="72" t="s">
+        <v>557</v>
+      </c>
+      <c r="L33" s="72" t="s">
+        <v>530</v>
+      </c>
+      <c r="M33" s="75" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="95" t="s">
+        <v>531</v>
+      </c>
+      <c r="B34" s="70" t="s">
+        <v>532</v>
+      </c>
+      <c r="C34" s="70" t="s">
+        <v>533</v>
+      </c>
+      <c r="D34" s="70" t="s">
+        <v>534</v>
+      </c>
+      <c r="E34" s="70" t="s">
+        <v>535</v>
+      </c>
+      <c r="F34" s="97" t="s">
+        <v>536</v>
+      </c>
+      <c r="G34" s="70" t="s">
+        <v>537</v>
+      </c>
+      <c r="H34" s="70" t="s">
+        <v>538</v>
+      </c>
+      <c r="I34" s="70" t="s">
+        <v>539</v>
+      </c>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70" t="s">
+        <v>540</v>
+      </c>
+      <c r="L34" s="70" t="s">
+        <v>541</v>
+      </c>
+      <c r="M34" s="98" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="95" t="s">
+        <v>558</v>
+      </c>
+      <c r="B35" s="70" t="s">
+        <v>559</v>
+      </c>
+      <c r="C35" s="70" t="s">
+        <v>560</v>
+      </c>
+      <c r="D35" s="70" t="s">
+        <v>561</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>562</v>
+      </c>
+      <c r="F35" s="70" t="s">
+        <v>563</v>
+      </c>
+      <c r="G35" s="70" t="s">
+        <v>564</v>
+      </c>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70" t="s">
+        <v>565</v>
+      </c>
+      <c r="J35" s="70" t="s">
+        <v>566</v>
+      </c>
+      <c r="K35" s="70" t="s">
+        <v>567</v>
+      </c>
+      <c r="L35" s="70" t="s">
+        <v>568</v>
+      </c>
+      <c r="M35" s="75" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B37" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C37" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D37" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E37" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F37" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G37" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H37" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I37" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J37" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K37" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L37" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M37" s="23" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>182</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F7" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="G7" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="54" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="J7" s="54" t="s">
-        <v>188</v>
-      </c>
-      <c r="K7" s="54" t="s">
-        <v>189</v>
-      </c>
-      <c r="L7" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="M7" s="55" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="K9" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="L9" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" s="52" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>194</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>198</v>
-      </c>
-      <c r="J10" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="K10" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="L10" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="M10" s="50" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="J11" s="43" t="s">
-        <v>211</v>
-      </c>
-      <c r="K11" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="M11" s="45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="M12" s="26" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="M14" s="26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="B15" s="60" t="s">
-        <v>237</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="M16" s="26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
-        <v>296</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="L19" s="59" t="s">
-        <v>307</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
-        <v>322</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D21" s="59" t="s">
-        <v>325</v>
-      </c>
-      <c r="E21" s="59" t="s">
-        <v>326</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="L21" s="59" t="s">
-        <v>333</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
-        <v>335</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="H22" s="62" t="s">
-        <v>342</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="M22" s="41" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>364</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>374</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>375</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>377</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="71" t="s">
-        <v>439</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>440</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>441</v>
-      </c>
-      <c r="D26" s="63" t="s">
-        <v>442</v>
-      </c>
-      <c r="E26" s="64" t="s">
-        <v>443</v>
-      </c>
-      <c r="F26" s="63" t="s">
-        <v>444</v>
-      </c>
-      <c r="G26" s="64" t="s">
-        <v>445</v>
-      </c>
-      <c r="H26" s="63" t="s">
-        <v>446</v>
-      </c>
-      <c r="I26" s="63" t="s">
-        <v>447</v>
-      </c>
-      <c r="J26" s="63" t="s">
-        <v>448</v>
-      </c>
-      <c r="K26" s="63" t="s">
-        <v>449</v>
-      </c>
-      <c r="L26" s="63" t="s">
-        <v>450</v>
-      </c>
-      <c r="M26" s="65" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="72" t="s">
-        <v>387</v>
-      </c>
-      <c r="B27" s="66" t="s">
-        <v>388</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>389</v>
-      </c>
-      <c r="D27" s="66" t="s">
-        <v>390</v>
-      </c>
-      <c r="E27" s="66" t="s">
-        <v>391</v>
-      </c>
-      <c r="F27" s="66" t="s">
-        <v>392</v>
-      </c>
-      <c r="G27" s="66" t="s">
-        <v>393</v>
-      </c>
-      <c r="H27" s="66" t="s">
-        <v>394</v>
-      </c>
-      <c r="I27" s="66" t="s">
-        <v>395</v>
-      </c>
-      <c r="J27" s="66" t="s">
-        <v>396</v>
-      </c>
-      <c r="K27" s="66" t="s">
-        <v>397</v>
-      </c>
-      <c r="L27" s="66" t="s">
-        <v>398</v>
-      </c>
-      <c r="M27" s="72" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
-        <v>400</v>
-      </c>
-      <c r="B28" s="67" t="s">
-        <v>401</v>
-      </c>
-      <c r="C28" s="66" t="s">
-        <v>402</v>
-      </c>
-      <c r="D28" s="66" t="s">
-        <v>403</v>
-      </c>
-      <c r="E28" s="66" t="s">
-        <v>404</v>
-      </c>
-      <c r="F28" s="66" t="s">
-        <v>405</v>
-      </c>
-      <c r="G28" s="67" t="s">
-        <v>406</v>
-      </c>
-      <c r="H28" s="66" t="s">
-        <v>407</v>
-      </c>
-      <c r="I28" s="66" t="s">
-        <v>408</v>
-      </c>
-      <c r="J28" s="67" t="s">
-        <v>409</v>
-      </c>
-      <c r="K28" s="66" t="s">
-        <v>410</v>
-      </c>
-      <c r="L28" s="66" t="s">
-        <v>411</v>
-      </c>
-      <c r="M28" s="75" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="73" t="s">
-        <v>413</v>
-      </c>
-      <c r="B29" s="66" t="s">
-        <v>414</v>
-      </c>
-      <c r="C29" s="66" t="s">
-        <v>415</v>
-      </c>
-      <c r="D29" s="66" t="s">
-        <v>416</v>
-      </c>
-      <c r="E29" s="66" t="s">
-        <v>417</v>
-      </c>
-      <c r="F29" s="66" t="s">
-        <v>418</v>
-      </c>
-      <c r="G29" s="66" t="s">
-        <v>419</v>
-      </c>
-      <c r="H29" s="66" t="s">
-        <v>420</v>
-      </c>
-      <c r="I29" s="66" t="s">
-        <v>421</v>
-      </c>
-      <c r="J29" s="66" t="s">
-        <v>422</v>
-      </c>
-      <c r="K29" s="66" t="s">
-        <v>423</v>
-      </c>
-      <c r="L29" s="66" t="s">
-        <v>424</v>
-      </c>
-      <c r="M29" s="73" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
-        <v>426</v>
-      </c>
-      <c r="B30" s="66" t="s">
-        <v>427</v>
-      </c>
-      <c r="C30" s="66" t="s">
-        <v>428</v>
-      </c>
-      <c r="D30" s="68" t="s">
-        <v>429</v>
-      </c>
-      <c r="E30" s="66" t="s">
-        <v>430</v>
-      </c>
-      <c r="F30" s="67" t="s">
-        <v>431</v>
-      </c>
-      <c r="G30" s="66" t="s">
-        <v>432</v>
-      </c>
-      <c r="H30" s="66" t="s">
-        <v>433</v>
-      </c>
-      <c r="I30" s="66" t="s">
-        <v>434</v>
-      </c>
-      <c r="J30" s="66" t="s">
-        <v>435</v>
-      </c>
-      <c r="K30" s="66" t="s">
-        <v>436</v>
-      </c>
-      <c r="L30" s="66" t="s">
-        <v>437</v>
-      </c>
-      <c r="M30" s="73" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
-        <v>452</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>453</v>
-      </c>
-      <c r="C31" s="68" t="s">
-        <v>454</v>
-      </c>
-      <c r="D31" s="67" t="s">
-        <v>455</v>
-      </c>
-      <c r="E31" s="66" t="s">
-        <v>456</v>
-      </c>
-      <c r="F31" s="66" t="s">
-        <v>457</v>
-      </c>
-      <c r="G31" s="66" t="s">
-        <v>458</v>
-      </c>
-      <c r="H31" s="66" t="s">
-        <v>459</v>
-      </c>
-      <c r="I31" s="66" t="s">
-        <v>460</v>
-      </c>
-      <c r="J31" s="66" t="s">
-        <v>461</v>
-      </c>
-      <c r="K31" s="66" t="s">
-        <v>462</v>
-      </c>
-      <c r="L31" s="66" t="s">
-        <v>463</v>
-      </c>
-      <c r="M31" s="75" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
-        <v>465</v>
-      </c>
-      <c r="B32" s="69" t="s">
-        <v>466</v>
-      </c>
-      <c r="C32" s="69" t="s">
-        <v>467</v>
-      </c>
-      <c r="D32" s="69" t="s">
-        <v>468</v>
-      </c>
-      <c r="E32" s="69" t="s">
-        <v>469</v>
-      </c>
-      <c r="F32" s="70" t="s">
-        <v>470</v>
-      </c>
-      <c r="G32" s="69" t="s">
-        <v>471</v>
-      </c>
-      <c r="H32" s="69" t="s">
-        <v>472</v>
-      </c>
-      <c r="I32" s="69" t="s">
-        <v>473</v>
-      </c>
-      <c r="J32" s="69" t="s">
-        <v>474</v>
-      </c>
-      <c r="K32" s="69" t="s">
-        <v>475</v>
-      </c>
-      <c r="L32" s="69" t="s">
-        <v>476</v>
-      </c>
-      <c r="M32" s="76" t="s">
-        <v>477</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3502,116 +4062,116 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="34"/>
       <c r="E2" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="34"/>
       <c r="E3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="34"/>
       <c r="E5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="34"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="34"/>
       <c r="E9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="34"/>
       <c r="E10" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="34" t="s">
         <v>165</v>
       </c>
       <c r="E12" t="s">
@@ -3619,38 +4179,38 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="34"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -3709,43 +4269,43 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L21" s="17" t="s">
+      <c r="L21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3830,57 +4390,57 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="31" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>136</v>
       </c>
       <c r="D6" t="s">
@@ -3888,35 +4448,35 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="31" t="s">
         <v>143</v>
       </c>
       <c r="D9" t="s">
@@ -3924,10 +4484,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="28" t="s">
         <v>142</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -3935,10 +4495,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="28" t="s">
         <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -3946,13 +4506,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="30" t="s">
         <v>149</v>
       </c>
       <c r="D12" t="s">
@@ -3960,46 +4520,46 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="30" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="30" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>121</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="30" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4021,4 +4581,189 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="69" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="68" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="68" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="68" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="69" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="69" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="69" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="69" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>506</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>